<commit_message>
Files Including DHTMLX Scheduler
</commit_message>
<xml_diff>
--- a/DatabaseDraft1.xlsx
+++ b/DatabaseDraft1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7035" tabRatio="312"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12000" windowHeight="5835" tabRatio="312"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
   <si>
     <t>id</t>
   </si>
@@ -86,15 +86,9 @@
     <t>EventTable</t>
   </si>
   <si>
-    <t>venueId</t>
-  </si>
-  <si>
     <t>serviceID</t>
   </si>
   <si>
-    <t>Date</t>
-  </si>
-  <si>
     <t>EndTime</t>
   </si>
   <si>
@@ -138,6 +132,9 @@
   </si>
   <si>
     <t>endDate</t>
+  </si>
+  <si>
+    <t>www</t>
   </si>
 </sst>
 </file>
@@ -183,10 +180,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -469,8 +466,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:V12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="V7" sqref="V7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -487,15 +484,15 @@
     <col min="16" max="16" width="5.7109375" customWidth="1"/>
     <col min="17" max="17" width="13" customWidth="1"/>
     <col min="18" max="18" width="9" customWidth="1"/>
-    <col min="19" max="19" width="7.7109375" customWidth="1"/>
+    <col min="19" max="19" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
     </row>
     <row r="3" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
@@ -505,61 +502,64 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" t="s">
         <v>4</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>2</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>3</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>17</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>5</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>6</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>7</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>8</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>9</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>10</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>11</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>12</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="R3" t="s">
         <v>13</v>
       </c>
-      <c r="R3" t="s">
+      <c r="S3" t="s">
         <v>14</v>
       </c>
-      <c r="S3" t="s">
+      <c r="T3" t="s">
         <v>15</v>
       </c>
-      <c r="T3" t="s">
+      <c r="U3" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="6" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="1"/>
+      <c r="D6" s="2"/>
       <c r="P6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="3:22" x14ac:dyDescent="0.25">
@@ -567,73 +567,67 @@
         <v>0</v>
       </c>
       <c r="D7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" t="s">
         <v>27</v>
       </c>
-      <c r="E7" t="s">
-        <v>28</v>
-      </c>
-      <c r="F7" t="s">
-        <v>29</v>
+      <c r="G7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7" t="s">
+        <v>21</v>
+      </c>
+      <c r="I7" t="s">
+        <v>34</v>
+      </c>
+      <c r="J7" t="s">
+        <v>35</v>
+      </c>
+      <c r="K7" t="s">
+        <v>23</v>
       </c>
       <c r="P7" t="s">
         <v>0</v>
       </c>
       <c r="Q7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="R7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="S7" t="s">
+        <v>30</v>
+      </c>
+      <c r="T7" t="s">
+        <v>31</v>
+      </c>
+      <c r="U7" t="s">
         <v>32</v>
       </c>
-      <c r="T7" t="s">
+      <c r="V7" t="s">
         <v>33</v>
-      </c>
-      <c r="U7" t="s">
-        <v>34</v>
-      </c>
-      <c r="V7" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="11" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="G11" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
+      <c r="G11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
     </row>
     <row r="12" spans="3:22" x14ac:dyDescent="0.25">
       <c r="G12" t="s">
         <v>0</v>
       </c>
       <c r="H12" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I12" t="s">
         <v>20</v>
-      </c>
-      <c r="J12" t="s">
-        <v>21</v>
-      </c>
-      <c r="K12" t="s">
-        <v>22</v>
-      </c>
-      <c r="L12" t="s">
-        <v>24</v>
-      </c>
-      <c r="M12" t="s">
-        <v>23</v>
-      </c>
-      <c r="N12" t="s">
-        <v>36</v>
-      </c>
-      <c r="O12" t="s">
-        <v>37</v>
-      </c>
-      <c r="P12" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>